<commit_message>
Modify master file downtime
</commit_message>
<xml_diff>
--- a/user_files/hilarytn/facility1/source1/line_3.xlsx
+++ b/user_files/hilarytn/facility1/source1/line_3.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,7 +507,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>7580109a-a8e0-4789-aaa6-bddca426b60e</t>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
         </is>
       </c>
       <c r="H2" s="3" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>7580109a-a8e0-4789-aaa6-bddca426b60e</t>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
         </is>
       </c>
       <c r="H3" s="3" t="n">
@@ -575,7 +575,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>7580109a-a8e0-4789-aaa6-bddca426b60e</t>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
         </is>
       </c>
       <c r="H4" s="3" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>7580109a-a8e0-4789-aaa6-bddca426b60e</t>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
         </is>
       </c>
       <c r="H5" s="3" t="n">
@@ -643,7 +643,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>7580109a-a8e0-4789-aaa6-bddca426b60e</t>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
         </is>
       </c>
       <c r="H6" s="3" t="n">
@@ -677,7 +677,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>7580109a-a8e0-4789-aaa6-bddca426b60e</t>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
         </is>
       </c>
       <c r="H7" s="3" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>7580109a-a8e0-4789-aaa6-bddca426b60e</t>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
         </is>
       </c>
       <c r="H8" s="3" t="n">
@@ -745,10 +745,282 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>7580109a-a8e0-4789-aaa6-bddca426b60e</t>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
         </is>
       </c>
       <c r="H9" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SEC Cl</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45271.36145825232</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>45271.36158556713</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PRI pH</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45271.68537890046</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>45271.68549464121</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>45271.68549475694</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>45271.68769383102</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>PRI pH&amp;rem SEC pH</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45271.6876965625</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>45271.68898128472</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>PRI pH&amp;rem SEC pH&amp;rem</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45271.68897129629</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>45271.68908703703</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45271.6890871875</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>45271.68920292824</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>PRI pH SEC pH</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45271.89825825232</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>45271.8996471412</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Line:3 Stage:1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>12/11/2023</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>PRI Cl&amp;pH</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>45272.09804105324</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>45272.09827253472</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>21accb77-0d31-426c-aa0c-0f4e7305dcd5</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>